<commit_message>
before changing listners class
</commit_message>
<xml_diff>
--- a/src/test/java/org/intuitiveapps/Kycee/Data/LoginTestData.xlsx
+++ b/src/test/java/org/intuitiveapps/Kycee/Data/LoginTestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
   <si>
     <t>Password</t>
   </si>
@@ -156,6 +156,24 @@
   </si>
   <si>
     <t>Ankunding</t>
+  </si>
+  <si>
+    <t>mileshodkiewicz@bsgdulpk.mailosaur.net</t>
+  </si>
+  <si>
+    <t>Miles</t>
+  </si>
+  <si>
+    <t>Hodkiewicz</t>
+  </si>
+  <si>
+    <t>sungreichel@bsgdulpk.mailosaur.net</t>
+  </si>
+  <si>
+    <t>Sung</t>
+  </si>
+  <si>
+    <t>Reichel</t>
   </si>
 </sst>
 </file>
@@ -535,10 +553,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="19.6640625"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="32.8203125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.703125"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.51171875"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.6328125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.359375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.046875"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="15.46875"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="24.59765625"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="26.765625"/>
@@ -548,42 +566,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -597,7 +615,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -611,7 +629,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -625,19 +643,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>9</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -649,59 +667,83 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="D7" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K7" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" t="s" s="0">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes done in Listners for parallel execution to work and add log in extent report
</commit_message>
<xml_diff>
--- a/src/test/java/org/intuitiveapps/Kycee/Data/LoginTestData.xlsx
+++ b/src/test/java/org/intuitiveapps/Kycee/Data/LoginTestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Password</t>
   </si>
@@ -174,6 +174,24 @@
   </si>
   <si>
     <t>Reichel</t>
+  </si>
+  <si>
+    <t>agathabauch@bsgdulpk.mailosaur.net</t>
+  </si>
+  <si>
+    <t>Agatha</t>
+  </si>
+  <si>
+    <t>Bauch</t>
+  </si>
+  <si>
+    <t>tatianawehner@bsgdulpk.mailosaur.net</t>
+  </si>
+  <si>
+    <t>Tatiana</t>
+  </si>
+  <si>
+    <t>Wehner</t>
   </si>
 </sst>
 </file>
@@ -671,16 +689,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s" s="0">
         <v>21</v>
@@ -706,16 +724,16 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s" s="0">
         <v>21</v>

</xml_diff>